<commit_message>
FileManage added, Converted JSON to C# Object
</commit_message>
<xml_diff>
--- a/SettingsHelperTest/Example_Settings_Calc_Sheet.xlsx
+++ b/SettingsHelperTest/Example_Settings_Calc_Sheet.xlsx
@@ -8,33 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tanner.Hollis\source\repos\SettingsHelper\SettingsHelperTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82314DFC-7E2F-488B-BDE4-A421B7203F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDF4784-4FF1-44F4-BC77-EDFF3C783502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C66D0D4-2E34-42F5-9A78-E4344EE2B48D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0C66D0D4-2E34-42F5-9A78-E4344EE2B48D}"/>
   </bookViews>
   <sheets>
     <sheet name="Calc Sheet" sheetId="2" r:id="rId1"/>
-    <sheet name="Supported Relay Types" sheetId="3" r:id="rId2"/>
+    <sheet name="Validation" sheetId="3" r:id="rId2"/>
     <sheet name="Title Sheet" sheetId="1" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet3" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet4" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="CTR">'Calc Sheet'!$C$32</definedName>
+    <definedName name="CTR">'Calc Sheet'!$C$33</definedName>
     <definedName name="CUSTCOMPANYNAME">'Calc Sheet'!$C$5</definedName>
     <definedName name="CustomerName">'Title Sheet'!$E$7</definedName>
     <definedName name="DATE">'Calc Sheet'!$C$2</definedName>
-    <definedName name="FREQ">'Calc Sheet'!$C$28</definedName>
+    <definedName name="FREQ">'Calc Sheet'!$C$29</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Title Sheet'!$A$1:$H$32</definedName>
     <definedName name="PROJECTNAME">'Calc Sheet'!$C$1</definedName>
-    <definedName name="PTR">'Calc Sheet'!$C$31</definedName>
+    <definedName name="PTR">'Calc Sheet'!$C$32</definedName>
+    <definedName name="RELAYNAME">'Calc Sheet'!$C$23</definedName>
     <definedName name="RELAYTYPE">'Calc Sheet'!$C$22</definedName>
-    <definedName name="Site_Rated_Capacity__kVA">'Calc Sheet'!$C$25</definedName>
-    <definedName name="System_Voltage__L_L__kV">'Calc Sheet'!$C$30</definedName>
-    <definedName name="VNOM">'Calc Sheet'!$C$35</definedName>
+    <definedName name="SITERATING_kVA">'Calc Sheet'!$C$26</definedName>
+    <definedName name="SYSTEMVOLTAGE_LL">'Calc Sheet'!$C$31</definedName>
+    <definedName name="VNOM">'Calc Sheet'!$C$36</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateCount="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -77,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="210">
   <si>
     <t>Mineral Gap</t>
   </si>
@@ -352,168 +353,9 @@
     <t>VNOM</t>
   </si>
   <si>
-    <t>27P1D</t>
-  </si>
-  <si>
-    <t>27P1P</t>
-  </si>
-  <si>
-    <t>27P2P</t>
-  </si>
-  <si>
-    <t>27P2D</t>
-  </si>
-  <si>
-    <t>59P1P</t>
-  </si>
-  <si>
-    <t>59P1D</t>
-  </si>
-  <si>
-    <t>59P2P</t>
-  </si>
-  <si>
-    <t>59P2D</t>
-  </si>
-  <si>
-    <t>81U1P</t>
-  </si>
-  <si>
-    <t>81U2P</t>
-  </si>
-  <si>
-    <t>81U1D</t>
-  </si>
-  <si>
-    <t>81U2D</t>
-  </si>
-  <si>
-    <t>81O2P</t>
-  </si>
-  <si>
-    <t>81O1D</t>
-  </si>
-  <si>
-    <t>81O1P</t>
-  </si>
-  <si>
-    <t>81O2D</t>
-  </si>
-  <si>
-    <t>50P1P</t>
-  </si>
-  <si>
-    <t>50P2P</t>
-  </si>
-  <si>
-    <t>50P3P</t>
-  </si>
-  <si>
-    <t>50P3D</t>
-  </si>
-  <si>
-    <t>50P4P</t>
-  </si>
-  <si>
-    <t>50P4D</t>
-  </si>
-  <si>
-    <t>50P2D</t>
-  </si>
-  <si>
-    <t>50G1P</t>
-  </si>
-  <si>
-    <t>50G1D</t>
-  </si>
-  <si>
-    <t>50D2P</t>
-  </si>
-  <si>
-    <t>50G2D</t>
-  </si>
-  <si>
-    <t>50G3P</t>
-  </si>
-  <si>
-    <t>50G3D</t>
-  </si>
-  <si>
-    <t>51P1P</t>
-  </si>
-  <si>
-    <t>51P1C</t>
-  </si>
-  <si>
-    <t>51P1R</t>
-  </si>
-  <si>
-    <t>51P1TD</t>
-  </si>
-  <si>
-    <t>51P1TM</t>
-  </si>
-  <si>
-    <t>51P1TA</t>
-  </si>
-  <si>
-    <t>51P2P</t>
-  </si>
-  <si>
-    <t>51P2C</t>
-  </si>
-  <si>
-    <t>51P2TD</t>
-  </si>
-  <si>
-    <t>51P2TM</t>
-  </si>
-  <si>
-    <t>51P2TA</t>
-  </si>
-  <si>
-    <t>51P2R</t>
-  </si>
-  <si>
     <t>Ground Time Overcurrent</t>
   </si>
   <si>
-    <t>51G1P</t>
-  </si>
-  <si>
-    <t>51G1C</t>
-  </si>
-  <si>
-    <t>51G1TD</t>
-  </si>
-  <si>
-    <t>51G1TM</t>
-  </si>
-  <si>
-    <t>51G1TA</t>
-  </si>
-  <si>
-    <t>51T1R</t>
-  </si>
-  <si>
-    <t>51G2P</t>
-  </si>
-  <si>
-    <t>51G2C</t>
-  </si>
-  <si>
-    <t>51G2TD</t>
-  </si>
-  <si>
-    <t>51G2TM</t>
-  </si>
-  <si>
-    <t>51G2TA</t>
-  </si>
-  <si>
-    <t>51G2R</t>
-  </si>
-  <si>
     <t>Power Elements</t>
   </si>
   <si>
@@ -526,39 +368,12 @@
     <t>Level 1 Power Type</t>
   </si>
   <si>
-    <t>PWR1P</t>
-  </si>
-  <si>
-    <t>PWR1D</t>
-  </si>
-  <si>
-    <t>3PWR1P</t>
-  </si>
-  <si>
-    <t>PWR1T</t>
-  </si>
-  <si>
     <t>Set to a percentage of site facility rating.</t>
   </si>
   <si>
     <t>+WATTS</t>
   </si>
   <si>
-    <t>PWR2P</t>
-  </si>
-  <si>
-    <t>3PWR2P</t>
-  </si>
-  <si>
-    <t>PWR2T</t>
-  </si>
-  <si>
-    <t>PWR2D</t>
-  </si>
-  <si>
-    <t>RLYTYPE</t>
-  </si>
-  <si>
     <t>SITERATING_kVA</t>
   </si>
   <si>
@@ -619,12 +434,6 @@
     <t>PRSCONTACTADDRESS2</t>
   </si>
   <si>
-    <t>59N1P</t>
-  </si>
-  <si>
-    <t>59N1D</t>
-  </si>
-  <si>
     <t>IEEE 1547 UV Setpoint Level 1</t>
   </si>
   <si>
@@ -674,6 +483,231 @@
   </si>
   <si>
     <t>Used in Open-Phase detection logic.</t>
+  </si>
+  <si>
+    <t>RELAYTYPE</t>
+  </si>
+  <si>
+    <t>RELAYNAME</t>
+  </si>
+  <si>
+    <t>Relay Name</t>
+  </si>
+  <si>
+    <t>Yes/No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Append Submittal Date?</t>
+  </si>
+  <si>
+    <t>Example Relay 1</t>
+  </si>
+  <si>
+    <t>V59P1P</t>
+  </si>
+  <si>
+    <t>V59P1D</t>
+  </si>
+  <si>
+    <t>V59P2P</t>
+  </si>
+  <si>
+    <t>V59P2D</t>
+  </si>
+  <si>
+    <t>V59N1P</t>
+  </si>
+  <si>
+    <t>V59N1D</t>
+  </si>
+  <si>
+    <t>V27P1P</t>
+  </si>
+  <si>
+    <t>V27P1D</t>
+  </si>
+  <si>
+    <t>V27P2P</t>
+  </si>
+  <si>
+    <t>V27P2D</t>
+  </si>
+  <si>
+    <t>F81U1P</t>
+  </si>
+  <si>
+    <t>F81U1D</t>
+  </si>
+  <si>
+    <t>F81U2P</t>
+  </si>
+  <si>
+    <t>F81U2D</t>
+  </si>
+  <si>
+    <t>F81O1P</t>
+  </si>
+  <si>
+    <t>F81O1D</t>
+  </si>
+  <si>
+    <t>F81O2P</t>
+  </si>
+  <si>
+    <t>F81O2D</t>
+  </si>
+  <si>
+    <t>I50P1P</t>
+  </si>
+  <si>
+    <t>I50P2D</t>
+  </si>
+  <si>
+    <t>I50P2P</t>
+  </si>
+  <si>
+    <t>I50P3P</t>
+  </si>
+  <si>
+    <t>I50P3D</t>
+  </si>
+  <si>
+    <t>I50P4P</t>
+  </si>
+  <si>
+    <t>I50P4D</t>
+  </si>
+  <si>
+    <t>I50G1P</t>
+  </si>
+  <si>
+    <t>I50G1D</t>
+  </si>
+  <si>
+    <t>I50D2P</t>
+  </si>
+  <si>
+    <t>I50G2D</t>
+  </si>
+  <si>
+    <t>I50G3P</t>
+  </si>
+  <si>
+    <t>I50G3D</t>
+  </si>
+  <si>
+    <t>I51P1P</t>
+  </si>
+  <si>
+    <t>I51P1C</t>
+  </si>
+  <si>
+    <t>I51P1TD</t>
+  </si>
+  <si>
+    <t>I51P1TM</t>
+  </si>
+  <si>
+    <t>I51P1TA</t>
+  </si>
+  <si>
+    <t>I51P1R</t>
+  </si>
+  <si>
+    <t>I51P2P</t>
+  </si>
+  <si>
+    <t>I51P2C</t>
+  </si>
+  <si>
+    <t>I51P2TD</t>
+  </si>
+  <si>
+    <t>I51P2TM</t>
+  </si>
+  <si>
+    <t>I51P2TA</t>
+  </si>
+  <si>
+    <t>I51P2R</t>
+  </si>
+  <si>
+    <t>I51G1P</t>
+  </si>
+  <si>
+    <t>I51G1C</t>
+  </si>
+  <si>
+    <t>I51G1TD</t>
+  </si>
+  <si>
+    <t>I51G1TM</t>
+  </si>
+  <si>
+    <t>I51G1TA</t>
+  </si>
+  <si>
+    <t>I51T1R</t>
+  </si>
+  <si>
+    <t>I51G2P</t>
+  </si>
+  <si>
+    <t>I51G2C</t>
+  </si>
+  <si>
+    <t>I51G2TD</t>
+  </si>
+  <si>
+    <t>I51G2TM</t>
+  </si>
+  <si>
+    <t>I51G2TA</t>
+  </si>
+  <si>
+    <t>I51G2R</t>
+  </si>
+  <si>
+    <t>PPWR1P</t>
+  </si>
+  <si>
+    <t>P3PWR1P</t>
+  </si>
+  <si>
+    <t>PPWR1T</t>
+  </si>
+  <si>
+    <t>PPWR1D</t>
+  </si>
+  <si>
+    <t>PPWR2P</t>
+  </si>
+  <si>
+    <t>P3PWR2P</t>
+  </si>
+  <si>
+    <t>PPWR2T</t>
+  </si>
+  <si>
+    <t>PPWR2D</t>
+  </si>
+  <si>
+    <t>Fwd/Rev</t>
+  </si>
+  <si>
+    <t>Fwd</t>
+  </si>
+  <si>
+    <t>Rev</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -681,7 +715,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000%"/>
+    <numFmt numFmtId="164" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -776,7 +810,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -821,13 +855,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -864,10 +911,24 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -878,19 +939,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1266,9 +1314,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDBF3620-65A2-4BED-8E75-DF5603F7533D}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:E117"/>
+  <dimension ref="A1:E118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
@@ -1283,7 +1331,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>164</v>
+        <v>102</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>2</v>
@@ -1294,7 +1342,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>103</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>29</v>
@@ -1310,7 +1358,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>104</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>31</v>
@@ -1321,7 +1369,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>105</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>21</v>
@@ -1332,7 +1380,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>106</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>22</v>
@@ -1343,7 +1391,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>171</v>
+        <v>109</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>23</v>
@@ -1354,7 +1402,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>172</v>
+        <v>110</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>24</v>
@@ -1365,7 +1413,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>169</v>
+        <v>107</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>25</v>
@@ -1376,7 +1424,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>170</v>
+        <v>108</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>26</v>
@@ -1395,7 +1443,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>173</v>
+        <v>111</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>30</v>
@@ -1406,7 +1454,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>175</v>
+        <v>113</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>27</v>
@@ -1417,7 +1465,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>174</v>
+        <v>112</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>28</v>
@@ -1426,9 +1474,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>178</v>
+        <v>116</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>32</v>
@@ -1437,9 +1485,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>117</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>33</v>
@@ -1448,9 +1496,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>176</v>
+        <v>114</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>34</v>
@@ -1459,9 +1507,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>177</v>
+        <v>115</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>35</v>
@@ -1470,794 +1518,800 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
+      <c r="C22" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>160</v>
-      </c>
-      <c r="B25" s="5" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C26" s="7">
         <v>3000</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>88</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B29" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C29" s="7">
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>89</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C30" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>163</v>
-      </c>
-      <c r="B30" s="5" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C31" s="7">
         <v>12.47</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B32" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C32" s="7">
         <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" s="10">
-        <f>C33/C34</f>
-        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>161</v>
+        <v>39</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="7">
-        <v>600</v>
+        <v>39</v>
+      </c>
+      <c r="C33" s="10">
+        <f>C34/C35</f>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>162</v>
+        <v>99</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C34" s="7">
-        <v>5</v>
+        <v>600</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>90</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B36" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="10" cm="1">
-        <f t="array" ref="C35">C30*1000/(SQRT(3)*PTR)</f>
+      <c r="C36" s="10" cm="1">
+        <f t="array" ref="C36">C31*1000/(SQRT(3)*PTR)</f>
         <v>119.99263094657724</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>92</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C38" s="10" cm="1">
-        <f t="array" ref="C38">D38*VNOM</f>
-        <v>105.59351523298797</v>
-      </c>
-      <c r="D38" s="14">
-        <v>0.88</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>91</v>
+        <v>149</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C39" s="8">
-        <v>120</v>
+        <v>48</v>
+      </c>
+      <c r="C39" s="10" cm="1">
+        <f t="array" ref="C39">D39*VNOM</f>
+        <v>105.59351523298797</v>
+      </c>
+      <c r="D39" s="14">
+        <v>0.88</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>93</v>
+        <v>150</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40" s="10">
-        <f>D40*VNOM</f>
-        <v>59.996315473288618</v>
-      </c>
-      <c r="D40" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>183</v>
+        <v>50</v>
+      </c>
+      <c r="C40" s="8">
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>94</v>
+        <v>151</v>
       </c>
       <c r="B41" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" s="10">
+        <f>D41*VNOM</f>
+        <v>59.996315473288618</v>
+      </c>
+      <c r="D41" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>152</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C41" s="8">
+      <c r="C42" s="8">
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="4" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>95</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C44" s="10">
-        <f>D44*VNOM</f>
-        <v>131.99189404123496</v>
-      </c>
-      <c r="D44" s="14">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>96</v>
+        <v>143</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C45" s="8">
+        <v>48</v>
+      </c>
+      <c r="C45" s="10">
+        <f>D45*VNOM</f>
+        <v>131.99189404123496</v>
+      </c>
+      <c r="D45" s="14">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E45" s="6" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>97</v>
+        <v>144</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C46" s="10">
-        <f>D46*VNOM</f>
-        <v>143.99115713589268</v>
-      </c>
-      <c r="D46" s="14">
-        <v>1.2</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>185</v>
+        <v>50</v>
+      </c>
+      <c r="C46" s="8">
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>98</v>
+        <v>145</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C47" s="8">
-        <v>12</v>
+        <v>49</v>
+      </c>
+      <c r="C47" s="10">
+        <f>D47*VNOM</f>
+        <v>143.99115713589268</v>
+      </c>
+      <c r="D47" s="14">
+        <v>1.2</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C48" s="10">
-        <f>D48*VNOM</f>
-        <v>11.999263094657724</v>
-      </c>
-      <c r="D48" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>198</v>
+        <v>51</v>
+      </c>
+      <c r="C48" s="8">
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="B49" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" s="10">
+        <f>D49*VNOM</f>
+        <v>11.999263094657724</v>
+      </c>
+      <c r="D49" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>148</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C49" s="10">
+      <c r="C50" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>99</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C52" s="10">
-        <f>D52*FREQ</f>
-        <v>59.499995999999996</v>
-      </c>
-      <c r="D52" s="23">
-        <v>0.99166659999999995</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>101</v>
+        <v>153</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C53" s="8">
-        <v>120</v>
+        <v>57</v>
+      </c>
+      <c r="C53" s="10">
+        <f>D53*FREQ</f>
+        <v>59.499995999999996</v>
+      </c>
+      <c r="D53" s="16">
+        <v>0.99166659999999995</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>100</v>
+        <v>154</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C54" s="10">
-        <f>D54*FREQ</f>
-        <v>58.999997999999998</v>
-      </c>
-      <c r="D54" s="23">
-        <v>0.98333329999999997</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>195</v>
+        <v>50</v>
+      </c>
+      <c r="C54" s="8">
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>102</v>
+        <v>155</v>
       </c>
       <c r="B55" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55" s="10">
+        <f>D55*FREQ</f>
+        <v>58.999997999999998</v>
+      </c>
+      <c r="D55" s="16">
+        <v>0.98333329999999997</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>156</v>
+      </c>
+      <c r="B56" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C55" s="8">
+      <c r="C56" s="8">
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>105</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C58" s="10">
-        <f>D58*FREQ</f>
-        <v>60.499998000000005</v>
-      </c>
-      <c r="D58" s="23">
-        <v>1.0083333000000001</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>104</v>
+        <v>157</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C59" s="8">
-        <v>120</v>
+        <v>57</v>
+      </c>
+      <c r="C59" s="10">
+        <f>D59*FREQ</f>
+        <v>60.499998000000005</v>
+      </c>
+      <c r="D59" s="16">
+        <v>1.0083333000000001</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>103</v>
+        <v>158</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C60" s="10">
-        <f>D60*FREQ</f>
-        <v>60.999995999999996</v>
-      </c>
-      <c r="D60" s="23">
-        <v>1.0166666</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>197</v>
+        <v>50</v>
+      </c>
+      <c r="C60" s="8">
+        <v>120</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>106</v>
+        <v>159</v>
       </c>
       <c r="B61" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C61" s="10">
+        <f>D61*FREQ</f>
+        <v>60.999995999999996</v>
+      </c>
+      <c r="D61" s="16">
+        <v>1.0166666</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>160</v>
+      </c>
+      <c r="B62" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C61" s="8">
+      <c r="C62" s="8">
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>107</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C64" s="8">
-        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>113</v>
+        <v>161</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="C65" s="8">
-        <v>0.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>108</v>
+        <v>162</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C66" s="8" t="s">
-        <v>72</v>
+        <v>50</v>
+      </c>
+      <c r="C66" s="8">
+        <v>0.5</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C67" s="8">
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>109</v>
+        <v>162</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C68" s="10">
-        <f>Site_Rated_Capacity__kVA*1000*D68/(SQRT(3)*CTR*System_Voltage__L_L__kV*1000)</f>
-        <v>1.3889741840969345</v>
-      </c>
-      <c r="D68" s="14">
-        <v>1.2</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>83</v>
+        <v>51</v>
+      </c>
+      <c r="C68" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>110</v>
+        <v>164</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C69" s="10">
-        <v>0</v>
+        <f>SITERATING_kVA*1000*D69/(SQRT(3)*CTR*SYSTEMVOLTAGE_LL*1000)</f>
+        <v>1.3889741840969345</v>
+      </c>
+      <c r="D69" s="14">
+        <v>1.2</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>111</v>
+        <v>165</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C70" s="10">
-        <f>Site_Rated_Capacity__kVA*1000*D70/(SQRT(3)*CTR*System_Voltage__L_L__kV*1000)</f>
-        <v>0.11574784867474454</v>
-      </c>
-      <c r="D70" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>73</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>112</v>
+        <v>166</v>
       </c>
       <c r="B71" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C71" s="10">
+        <f>SITERATING_kVA*1000*D71/(SQRT(3)*CTR*SYSTEMVOLTAGE_LL*1000)</f>
+        <v>0.11574784867474454</v>
+      </c>
+      <c r="D71" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>167</v>
+      </c>
+      <c r="B72" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C71" s="10">
+      <c r="C72" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B73" s="4" t="s">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>114</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C74" s="8">
-        <v>5.16</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>115</v>
+        <v>168</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="C75" s="8">
-        <v>0.01</v>
+        <v>5.16</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>116</v>
+        <v>169</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C76" s="8" t="s">
-        <v>72</v>
+        <v>50</v>
+      </c>
+      <c r="C76" s="8">
+        <v>0.01</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>117</v>
+        <v>170</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C77" s="8">
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>118</v>
+        <v>171</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C78" s="10">
-        <f>Site_Rated_Capacity__kVA*1000*D78/(SQRT(3)*CTR*System_Voltage__L_L__kV*1000)</f>
-        <v>1.1574784867474455</v>
-      </c>
-      <c r="D78" s="14">
-        <v>1</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>83</v>
+        <v>51</v>
+      </c>
+      <c r="C78" s="8">
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>119</v>
+        <v>172</v>
       </c>
       <c r="B79" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C79" s="10">
+        <f>SITERATING_kVA*1000*D79/(SQRT(3)*CTR*SYSTEMVOLTAGE_LL*1000)</f>
+        <v>1.1574784867474455</v>
+      </c>
+      <c r="D79" s="14">
+        <v>1</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>173</v>
+      </c>
+      <c r="B80" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C79" s="10">
+      <c r="C80" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B80" s="5"/>
-      <c r="C80" s="11"/>
-      <c r="D80" s="12"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B81" s="4" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="5"/>
+      <c r="C81" s="11"/>
+      <c r="D81" s="12"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>120</v>
-      </c>
-      <c r="B82" s="5" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>174</v>
+      </c>
+      <c r="B83" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C82" s="7">
+      <c r="C83" s="7">
         <v>1.32</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>121</v>
-      </c>
-      <c r="B83" s="5" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>175</v>
+      </c>
+      <c r="B84" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C83" s="7" t="s">
+      <c r="C84" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>123</v>
-      </c>
-      <c r="B84" s="5" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>176</v>
+      </c>
+      <c r="B85" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C84" s="7">
+      <c r="C85" s="7">
         <v>0.66</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>124</v>
-      </c>
-      <c r="B85" s="5" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>177</v>
+      </c>
+      <c r="B86" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="C85" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>125</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>78</v>
       </c>
       <c r="C86" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>122</v>
+        <v>178</v>
       </c>
       <c r="B87" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C87" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>179</v>
+      </c>
+      <c r="B88" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C87" s="7" t="s">
+      <c r="C88" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>126</v>
-      </c>
-      <c r="B88" s="5" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>180</v>
+      </c>
+      <c r="B89" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C88" s="7">
+      <c r="C89" s="7">
         <v>1.32</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>127</v>
-      </c>
-      <c r="B89" s="5" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>181</v>
+      </c>
+      <c r="B90" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C89" s="7" t="s">
+      <c r="C90" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>128</v>
-      </c>
-      <c r="B90" s="5" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>182</v>
+      </c>
+      <c r="B91" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C90" s="7">
+      <c r="C91" s="7">
         <v>0.66</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>129</v>
-      </c>
-      <c r="B91" s="5" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>183</v>
+      </c>
+      <c r="B92" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="C91" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>130</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="C92" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>131</v>
+        <v>184</v>
       </c>
       <c r="B93" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C93" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>185</v>
+      </c>
+      <c r="B94" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C93" s="7" t="s">
+      <c r="C94" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B94" s="5"/>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B95" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>133</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C96" s="7">
-        <v>1.32</v>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B95" s="5"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B96" s="4" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>134</v>
+        <v>186</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C97" s="7" t="s">
-        <v>80</v>
+        <v>63</v>
+      </c>
+      <c r="C97" s="7">
+        <v>1.32</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>135</v>
+        <v>187</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C98" s="7">
-        <v>0.66</v>
+        <v>75</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>136</v>
+        <v>188</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C99" s="7">
-        <v>0</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>137</v>
+        <v>189</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C100" s="7">
         <v>0</v>
@@ -2265,65 +2319,65 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>138</v>
+        <v>190</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C101" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
+      </c>
+      <c r="C101" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>139</v>
+        <v>191</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>140</v>
+        <v>192</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>141</v>
+        <v>193</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C104" s="7">
-        <v>0.66</v>
+        <v>84</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>142</v>
+        <v>194</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C105" s="7">
-        <v>0</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>143</v>
+        <v>195</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C106" s="7">
         <v>0</v>
@@ -2331,113 +2385,124 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>144</v>
+        <v>196</v>
       </c>
       <c r="B107" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C107" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>197</v>
+      </c>
+      <c r="B108" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C107" s="7" t="s">
+      <c r="C108" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B109" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>149</v>
-      </c>
-      <c r="B110" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C110" s="7" t="s">
-        <v>72</v>
+      <c r="B110" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>151</v>
+        <v>198</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C111" s="24">
-        <f>Site_Rated_Capacity__kVA*1000*D111/(PTR*CTR)</f>
-        <v>437.5</v>
-      </c>
-      <c r="D111" s="14">
-        <v>1.05</v>
-      </c>
-      <c r="E111" s="6" t="s">
-        <v>153</v>
+        <v>93</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>152</v>
+        <v>199</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C112" s="13" t="s">
-        <v>154</v>
+        <v>94</v>
+      </c>
+      <c r="C112" s="10">
+        <f>SITERATING_kVA*1000*D112/(PTR*CTR)</f>
+        <v>437.5</v>
+      </c>
+      <c r="D112" s="14">
+        <v>1.05</v>
+      </c>
+      <c r="E112" s="6" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C113" s="25">
-        <v>16000</v>
+        <v>95</v>
+      </c>
+      <c r="C113" s="13" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>155</v>
+        <v>201</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="C114" s="7" t="s">
-        <v>72</v>
+        <v>50</v>
+      </c>
+      <c r="C114" s="17">
+        <v>16000</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>156</v>
+        <v>202</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C115" s="8">
-        <f>Site_Rated_Capacity__kVA*1000*D115/(PTR*CTR)</f>
-        <v>0</v>
+        <v>122</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>157</v>
+        <v>203</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="C116" s="13" t="s">
-        <v>154</v>
+        <v>123</v>
+      </c>
+      <c r="C116" s="8">
+        <f>SITERATING_kVA*1000*D116/(PTR*CTR)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>158</v>
+        <v>204</v>
       </c>
       <c r="B117" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C117" s="13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>205</v>
+      </c>
+      <c r="B118" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C117" s="8">
+      <c r="C118" s="8">
         <v>16000</v>
       </c>
     </row>
@@ -2450,12 +2515,18 @@
   <pageSetup orientation="portrait" r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7DCEE676-09AB-437A-9105-868C70093386}">
           <x14:formula1>
-            <xm:f>'Supported Relay Types'!$A$2:$A$30</xm:f>
+            <xm:f>Validation!$A$2:$A$30</xm:f>
           </x14:formula1>
           <xm:sqref>C22</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DD449E96-625C-4E32-9997-00AEFCE41B1D}">
+          <x14:formula1>
+            <xm:f>Validation!$B$2:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>D23</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2465,10 +2536,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66BF056A-9FA2-43E8-BA55-827BD43044C1}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2476,33 +2547,55 @@
     <col min="1" max="1" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="B2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="B3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="C4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>192</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2537,198 +2630,190 @@
       <c r="H2" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="18" t="str">
+      <c r="B5" s="24" t="str">
         <f>_xlfn.CONCAT(RELAYTYPE," RELAY")</f>
         <v>SEL 351-7 RELAY</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="20" t="s">
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="20" t="s">
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="20">
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="26">
         <v>20211208</v>
       </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
     </row>
     <row r="22" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="C27:F27"/>
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C20:F20"/>
@@ -2744,6 +2829,14 @@
     <mergeCell ref="C14:F14"/>
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="C27:F27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C19" r:id="rId1" xr:uid="{38A204EC-D754-48E5-83D4-E0733367D728}"/>

</xml_diff>